<commit_message>
form fix (fix boxes)
</commit_message>
<xml_diff>
--- a/APIFinal/templates/various-form.xlsx
+++ b/APIFinal/templates/various-form.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\source\repos\API\APIFinal\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C76BBA2-5F5B-497A-8B20-8E7BC1011A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C81AF93-6624-4E91-B8E3-3FB40D1AD7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13290" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PAR" sheetId="14" r:id="rId1"/>
@@ -341,9 +341,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -471,6 +471,12 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -987,11 +993,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="17" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="162">
+  <cellXfs count="163">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1089,7 +1095,7 @@
     <xf numFmtId="4" fontId="7" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1">
@@ -1197,16 +1203,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="32" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="29" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1">
@@ -1248,6 +1254,9 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1290,9 +1299,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1329,6 +1335,9 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1437,8 +1446,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2968,7 +2977,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>87630</xdr:colOff>
+      <xdr:colOff>46808</xdr:colOff>
       <xdr:row>4</xdr:row>
       <xdr:rowOff>208280</xdr:rowOff>
     </xdr:to>
@@ -4322,26 +4331,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="25.5">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="102" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
     </row>
     <row r="4" spans="1:7" ht="16.5">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
     </row>
     <row r="6" spans="1:7">
       <c r="E6" s="26" t="s">
@@ -4720,12 +4729,12 @@
         <v>32</v>
       </c>
       <c r="C41" s="73"/>
-      <c r="D41" s="102" t="s">
+      <c r="D41" s="103" t="s">
         <v>33</v>
       </c>
-      <c r="E41" s="103"/>
-      <c r="F41" s="103"/>
-      <c r="G41" s="104"/>
+      <c r="E41" s="104"/>
+      <c r="F41" s="104"/>
+      <c r="G41" s="105"/>
     </row>
     <row r="42" spans="1:7" ht="16.5">
       <c r="A42" s="74"/>
@@ -4736,8 +4745,8 @@
       <c r="D42" s="74" t="s">
         <v>35</v>
       </c>
-      <c r="E42" s="99"/>
-      <c r="F42" s="99"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="100"/>
       <c r="G42" s="73"/>
     </row>
     <row r="43" spans="1:7" ht="16.5">
@@ -4786,12 +4795,12 @@
         <v>38</v>
       </c>
       <c r="C47" s="73"/>
-      <c r="D47" s="105" t="s">
+      <c r="D47" s="106" t="s">
         <v>33</v>
       </c>
-      <c r="E47" s="106"/>
-      <c r="F47" s="106"/>
-      <c r="G47" s="107"/>
+      <c r="E47" s="107"/>
+      <c r="F47" s="107"/>
+      <c r="G47" s="108"/>
     </row>
     <row r="48" spans="1:7" ht="16.5">
       <c r="A48" s="74"/>
@@ -4799,10 +4808,10 @@
         <v>39</v>
       </c>
       <c r="C48" s="73"/>
-      <c r="D48" s="98"/>
-      <c r="E48" s="99"/>
-      <c r="F48" s="99"/>
-      <c r="G48" s="100"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="100"/>
+      <c r="F48" s="100"/>
+      <c r="G48" s="101"/>
     </row>
     <row r="49" spans="1:7" ht="16.5">
       <c r="A49" s="74"/>
@@ -4857,77 +4866,81 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A2:J101"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="1" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.7109375" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="7.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.28515625" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.42578125" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:10">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="107" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="106"/>
-      <c r="C2" s="106"/>
-      <c r="D2" s="106"/>
-      <c r="E2" s="106"/>
-      <c r="F2" s="106"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="106"/>
-      <c r="J2" s="106"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
+      <c r="E2" s="107"/>
+      <c r="F2" s="107"/>
+      <c r="G2" s="107"/>
+      <c r="H2" s="107"/>
+      <c r="I2" s="107"/>
+      <c r="J2" s="107"/>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="106" t="s">
+      <c r="A3" s="107" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="106"/>
-      <c r="C3" s="106"/>
-      <c r="D3" s="106"/>
-      <c r="E3" s="106"/>
-      <c r="F3" s="106"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="106"/>
-      <c r="J3" s="106"/>
+      <c r="B3" s="107"/>
+      <c r="C3" s="107"/>
+      <c r="D3" s="107"/>
+      <c r="E3" s="107"/>
+      <c r="F3" s="107"/>
+      <c r="G3" s="107"/>
+      <c r="H3" s="107"/>
+      <c r="I3" s="107"/>
+      <c r="J3" s="107"/>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="106"/>
-      <c r="B4" s="106"/>
-      <c r="C4" s="106"/>
-      <c r="D4" s="106"/>
-      <c r="E4" s="106"/>
-      <c r="F4" s="106"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="106"/>
-      <c r="J4" s="106"/>
+      <c r="A4" s="107"/>
+      <c r="B4" s="107"/>
+      <c r="C4" s="107"/>
+      <c r="D4" s="107"/>
+      <c r="E4" s="107"/>
+      <c r="F4" s="107"/>
+      <c r="G4" s="107"/>
+      <c r="H4" s="107"/>
+      <c r="I4" s="107"/>
+      <c r="J4" s="107"/>
     </row>
     <row r="5" spans="1:10" ht="18">
-      <c r="A5" s="126" t="s">
+      <c r="A5" s="127" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
-      <c r="G5" s="126"/>
-      <c r="H5" s="126"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
+      <c r="B5" s="127"/>
+      <c r="C5" s="127"/>
+      <c r="D5" s="127"/>
+      <c r="E5" s="127"/>
+      <c r="F5" s="127"/>
+      <c r="G5" s="127"/>
+      <c r="H5" s="127"/>
+      <c r="I5" s="127"/>
+      <c r="J5" s="127"/>
     </row>
     <row r="6" spans="1:10" ht="18">
       <c r="A6" s="75"/>
@@ -4984,16 +4997,16 @@
       <c r="J10" s="76"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="109" t="s">
+      <c r="A11" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="111" t="s">
+      <c r="B11" s="112" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="127" t="s">
+      <c r="C11" s="128" t="s">
         <v>47</v>
       </c>
-      <c r="D11" s="128"/>
+      <c r="D11" s="129"/>
       <c r="E11" s="115" t="s">
         <v>48</v>
       </c>
@@ -5008,8 +5021,8 @@
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="110"/>
-      <c r="B12" s="112"/>
+      <c r="A12" s="111"/>
+      <c r="B12" s="162"/>
       <c r="C12" s="78" t="s">
         <v>51</v>
       </c>
@@ -5040,10 +5053,10 @@
       <c r="B14" s="80"/>
       <c r="C14" s="81"/>
       <c r="D14" s="81"/>
-      <c r="E14" s="125"/>
-      <c r="F14" s="125"/>
-      <c r="G14" s="125"/>
-      <c r="H14" s="125"/>
+      <c r="E14" s="126"/>
+      <c r="F14" s="126"/>
+      <c r="G14" s="126"/>
+      <c r="H14" s="126"/>
       <c r="I14" s="80"/>
       <c r="J14" s="80"/>
     </row>
@@ -5355,18 +5368,18 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="88"/>
-      <c r="B40" s="108" t="s">
+      <c r="B40" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="108"/>
-      <c r="D40" s="108"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="109"/>
       <c r="E40" s="90"/>
       <c r="F40" s="89"/>
-      <c r="G40" s="108" t="s">
+      <c r="G40" s="109" t="s">
         <v>56</v>
       </c>
-      <c r="H40" s="108"/>
-      <c r="I40" s="108"/>
+      <c r="H40" s="109"/>
+      <c r="I40" s="109"/>
       <c r="J40" s="90"/>
     </row>
     <row r="41" spans="1:10">
@@ -5409,18 +5422,18 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="88"/>
-      <c r="B44" s="108" t="s">
+      <c r="B44" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="C44" s="108"/>
-      <c r="D44" s="108"/>
+      <c r="C44" s="109"/>
+      <c r="D44" s="109"/>
       <c r="E44" s="90"/>
       <c r="F44" s="89"/>
-      <c r="G44" s="108" t="s">
+      <c r="G44" s="109" t="s">
         <v>58</v>
       </c>
-      <c r="H44" s="108"/>
-      <c r="I44" s="108"/>
+      <c r="H44" s="109"/>
+      <c r="I44" s="109"/>
       <c r="J44" s="90"/>
     </row>
     <row r="45" spans="1:10">
@@ -5461,18 +5474,18 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="88"/>
-      <c r="B48" s="108" t="s">
+      <c r="B48" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="C48" s="108"/>
-      <c r="D48" s="108"/>
+      <c r="C48" s="109"/>
+      <c r="D48" s="109"/>
       <c r="E48" s="90"/>
       <c r="F48" s="89"/>
-      <c r="G48" s="108" t="s">
+      <c r="G48" s="109" t="s">
         <v>59</v>
       </c>
-      <c r="H48" s="108"/>
-      <c r="I48" s="108"/>
+      <c r="H48" s="109"/>
+      <c r="I48" s="109"/>
       <c r="J48" s="90"/>
     </row>
     <row r="49" spans="1:10">
@@ -6157,8 +6170,9 @@
     <mergeCell ref="E35:H35"/>
     <mergeCell ref="B39:D39"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.74803149606299213" right="0.74803149606299213" top="0.74803149606299213" bottom="0.74803149606299213" header="0.29921259842519687" footer="0.29921259842519687"/>
+  <pageSetup paperSize="9" scale="81" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -6166,7 +6180,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
@@ -6182,37 +6196,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="25.5">
-      <c r="A2" s="101" t="s">
+      <c r="A2" s="102" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="101"/>
-      <c r="C2" s="101"/>
-      <c r="D2" s="101"/>
-      <c r="E2" s="101"/>
-      <c r="F2" s="101"/>
-      <c r="G2" s="101"/>
+      <c r="B2" s="102"/>
+      <c r="C2" s="102"/>
+      <c r="D2" s="102"/>
+      <c r="E2" s="102"/>
+      <c r="F2" s="102"/>
+      <c r="G2" s="102"/>
     </row>
     <row r="4" spans="1:7" ht="16.5">
-      <c r="A4" s="99" t="s">
+      <c r="A4" s="100" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="99"/>
-      <c r="C4" s="99"/>
-      <c r="D4" s="99"/>
-      <c r="E4" s="99"/>
-      <c r="F4" s="99"/>
-      <c r="G4" s="99"/>
+      <c r="B4" s="100"/>
+      <c r="C4" s="100"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
     </row>
     <row r="5" spans="1:7" ht="16.5">
-      <c r="A5" s="99" t="s">
+      <c r="A5" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="99"/>
-      <c r="C5" s="99"/>
-      <c r="D5" s="99"/>
-      <c r="E5" s="99"/>
-      <c r="F5" s="99"/>
-      <c r="G5" s="99"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="100"/>
+      <c r="E5" s="100"/>
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
     </row>
     <row r="6" spans="1:7">
       <c r="E6" s="26"/>
@@ -6243,7 +6257,7 @@
     <row r="9" spans="1:7" ht="16.5">
       <c r="A9" s="33"/>
       <c r="B9" s="34"/>
-      <c r="C9" s="161"/>
+      <c r="C9" s="98"/>
       <c r="D9" s="35"/>
       <c r="E9" s="36"/>
       <c r="F9" s="37"/>
@@ -6506,26 +6520,26 @@
       <c r="G34" s="73"/>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" s="105"/>
-      <c r="B35" s="106"/>
-      <c r="C35" s="107"/>
-      <c r="D35" s="102" t="s">
+      <c r="A35" s="106"/>
+      <c r="B35" s="107"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="103" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="106"/>
-      <c r="F35" s="106"/>
-      <c r="G35" s="107"/>
+      <c r="E35" s="107"/>
+      <c r="F35" s="107"/>
+      <c r="G35" s="108"/>
     </row>
     <row r="36" spans="1:7" ht="16.5">
-      <c r="A36" s="98"/>
-      <c r="B36" s="99"/>
-      <c r="C36" s="100"/>
-      <c r="D36" s="98" t="s">
+      <c r="A36" s="99"/>
+      <c r="B36" s="100"/>
+      <c r="C36" s="101"/>
+      <c r="D36" s="99" t="s">
         <v>64</v>
       </c>
-      <c r="E36" s="99"/>
-      <c r="F36" s="99"/>
-      <c r="G36" s="100"/>
+      <c r="E36" s="100"/>
+      <c r="F36" s="100"/>
+      <c r="G36" s="101"/>
     </row>
     <row r="37" spans="1:7" ht="16.5">
       <c r="A37" s="48"/>
@@ -6559,35 +6573,35 @@
       <c r="G39" s="73"/>
     </row>
     <row r="40" spans="1:7" ht="16.5">
-      <c r="A40" s="129"/>
-      <c r="B40" s="126"/>
-      <c r="C40" s="130"/>
+      <c r="A40" s="130"/>
+      <c r="B40" s="127"/>
+      <c r="C40" s="131"/>
       <c r="D40" s="74"/>
       <c r="E40" s="36"/>
       <c r="F40" s="36"/>
       <c r="G40" s="73"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="129"/>
-      <c r="B41" s="126"/>
-      <c r="C41" s="130"/>
-      <c r="D41" s="105" t="s">
+      <c r="A41" s="130"/>
+      <c r="B41" s="127"/>
+      <c r="C41" s="131"/>
+      <c r="D41" s="106" t="s">
         <v>66</v>
       </c>
-      <c r="E41" s="106"/>
-      <c r="F41" s="106"/>
-      <c r="G41" s="107"/>
+      <c r="E41" s="107"/>
+      <c r="F41" s="107"/>
+      <c r="G41" s="108"/>
     </row>
     <row r="42" spans="1:7" ht="16.5">
       <c r="A42" s="74"/>
       <c r="B42" s="36"/>
       <c r="C42" s="73"/>
-      <c r="D42" s="98" t="s">
+      <c r="D42" s="99" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="99"/>
-      <c r="F42" s="99"/>
-      <c r="G42" s="100"/>
+      <c r="E42" s="100"/>
+      <c r="F42" s="100"/>
+      <c r="G42" s="101"/>
     </row>
     <row r="43" spans="1:7" ht="16.5">
       <c r="A43" s="48"/>
@@ -6659,10 +6673,10 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="155" t="s">
+      <c r="H1" s="156" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="155"/>
+      <c r="I1" s="156"/>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1"/>
@@ -6676,17 +6690,17 @@
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="18.75">
-      <c r="A3" s="156" t="s">
+      <c r="A3" s="157" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="156"/>
-      <c r="C3" s="156"/>
-      <c r="D3" s="156"/>
-      <c r="E3" s="156"/>
-      <c r="F3" s="156"/>
-      <c r="G3" s="156"/>
-      <c r="H3" s="156"/>
-      <c r="I3" s="156"/>
+      <c r="B3" s="157"/>
+      <c r="C3" s="157"/>
+      <c r="D3" s="157"/>
+      <c r="E3" s="157"/>
+      <c r="F3" s="157"/>
+      <c r="G3" s="157"/>
+      <c r="H3" s="157"/>
+      <c r="I3" s="157"/>
     </row>
     <row r="4" spans="1:9" ht="18.75">
       <c r="A4" s="2"/>
@@ -6700,15 +6714,15 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" spans="1:9" ht="15.75">
-      <c r="A5" s="157"/>
-      <c r="B5" s="157"/>
-      <c r="C5" s="157"/>
-      <c r="D5" s="157"/>
-      <c r="E5" s="157"/>
-      <c r="F5" s="157"/>
-      <c r="G5" s="157"/>
-      <c r="H5" s="157"/>
-      <c r="I5" s="157"/>
+      <c r="A5" s="158"/>
+      <c r="B5" s="158"/>
+      <c r="C5" s="158"/>
+      <c r="D5" s="158"/>
+      <c r="E5" s="158"/>
+      <c r="F5" s="158"/>
+      <c r="G5" s="158"/>
+      <c r="H5" s="158"/>
+      <c r="I5" s="158"/>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="3" t="s">
@@ -6719,11 +6733,11 @@
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="144" t="s">
+      <c r="G6" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="144"/>
-      <c r="I6" s="144"/>
+      <c r="H6" s="145"/>
+      <c r="I6" s="145"/>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" s="1"/>
@@ -6843,309 +6857,309 @@
       <c r="I15" s="22"/>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="134" t="s">
+      <c r="A16" s="135" t="s">
         <v>81</v>
       </c>
-      <c r="B16" s="138" t="s">
+      <c r="B16" s="139" t="s">
         <v>82</v>
       </c>
-      <c r="C16" s="139"/>
-      <c r="D16" s="138" t="s">
+      <c r="C16" s="140"/>
+      <c r="D16" s="139" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="141"/>
-      <c r="F16" s="141"/>
-      <c r="G16" s="139"/>
-      <c r="H16" s="134" t="s">
+      <c r="E16" s="142"/>
+      <c r="F16" s="142"/>
+      <c r="G16" s="140"/>
+      <c r="H16" s="135" t="s">
         <v>47</v>
       </c>
-      <c r="I16" s="136" t="s">
+      <c r="I16" s="137" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="135"/>
-      <c r="B17" s="140"/>
-      <c r="C17" s="137"/>
-      <c r="D17" s="140"/>
-      <c r="E17" s="142"/>
-      <c r="F17" s="142"/>
-      <c r="G17" s="137"/>
-      <c r="H17" s="135"/>
-      <c r="I17" s="137"/>
+      <c r="A17" s="136"/>
+      <c r="B17" s="141"/>
+      <c r="C17" s="138"/>
+      <c r="D17" s="141"/>
+      <c r="E17" s="143"/>
+      <c r="F17" s="143"/>
+      <c r="G17" s="138"/>
+      <c r="H17" s="136"/>
+      <c r="I17" s="138"/>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="10"/>
-      <c r="B18" s="158"/>
-      <c r="C18" s="159"/>
-      <c r="D18" s="158"/>
-      <c r="E18" s="160"/>
-      <c r="F18" s="160"/>
-      <c r="G18" s="159"/>
+      <c r="B18" s="159"/>
+      <c r="C18" s="160"/>
+      <c r="D18" s="159"/>
+      <c r="E18" s="161"/>
+      <c r="F18" s="161"/>
+      <c r="G18" s="160"/>
       <c r="H18" s="10"/>
       <c r="I18" s="23"/>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" s="10"/>
-      <c r="B19" s="151"/>
-      <c r="C19" s="133"/>
-      <c r="D19" s="151"/>
-      <c r="E19" s="132"/>
-      <c r="F19" s="132"/>
-      <c r="G19" s="133"/>
+      <c r="B19" s="152"/>
+      <c r="C19" s="134"/>
+      <c r="D19" s="152"/>
+      <c r="E19" s="133"/>
+      <c r="F19" s="133"/>
+      <c r="G19" s="134"/>
       <c r="H19" s="10"/>
       <c r="I19" s="23"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="10"/>
-      <c r="B20" s="151"/>
-      <c r="C20" s="133"/>
-      <c r="D20" s="151"/>
-      <c r="E20" s="132"/>
-      <c r="F20" s="132"/>
-      <c r="G20" s="133"/>
+      <c r="B20" s="152"/>
+      <c r="C20" s="134"/>
+      <c r="D20" s="152"/>
+      <c r="E20" s="133"/>
+      <c r="F20" s="133"/>
+      <c r="G20" s="134"/>
       <c r="H20" s="10"/>
       <c r="I20" s="23"/>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="10"/>
-      <c r="B21" s="151"/>
-      <c r="C21" s="133"/>
-      <c r="D21" s="151"/>
-      <c r="E21" s="132"/>
-      <c r="F21" s="132"/>
-      <c r="G21" s="133"/>
+      <c r="B21" s="152"/>
+      <c r="C21" s="134"/>
+      <c r="D21" s="152"/>
+      <c r="E21" s="133"/>
+      <c r="F21" s="133"/>
+      <c r="G21" s="134"/>
       <c r="H21" s="10"/>
       <c r="I21" s="23"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="10"/>
-      <c r="B22" s="151"/>
-      <c r="C22" s="133"/>
-      <c r="D22" s="151"/>
-      <c r="E22" s="132"/>
-      <c r="F22" s="132"/>
-      <c r="G22" s="133"/>
+      <c r="B22" s="152"/>
+      <c r="C22" s="134"/>
+      <c r="D22" s="152"/>
+      <c r="E22" s="133"/>
+      <c r="F22" s="133"/>
+      <c r="G22" s="134"/>
       <c r="H22" s="10"/>
       <c r="I22" s="23"/>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" s="10"/>
-      <c r="B23" s="151"/>
-      <c r="C23" s="133"/>
-      <c r="D23" s="151"/>
-      <c r="E23" s="132"/>
-      <c r="F23" s="132"/>
-      <c r="G23" s="133"/>
+      <c r="B23" s="152"/>
+      <c r="C23" s="134"/>
+      <c r="D23" s="152"/>
+      <c r="E23" s="133"/>
+      <c r="F23" s="133"/>
+      <c r="G23" s="134"/>
       <c r="H23" s="10"/>
       <c r="I23" s="23"/>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" s="10"/>
-      <c r="B24" s="151"/>
-      <c r="C24" s="133"/>
-      <c r="D24" s="151"/>
-      <c r="E24" s="132"/>
-      <c r="F24" s="132"/>
-      <c r="G24" s="133"/>
+      <c r="B24" s="152"/>
+      <c r="C24" s="134"/>
+      <c r="D24" s="152"/>
+      <c r="E24" s="133"/>
+      <c r="F24" s="133"/>
+      <c r="G24" s="134"/>
       <c r="H24" s="10"/>
       <c r="I24" s="23"/>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" s="10"/>
-      <c r="B25" s="151"/>
-      <c r="C25" s="133"/>
-      <c r="D25" s="151"/>
-      <c r="E25" s="132"/>
-      <c r="F25" s="132"/>
-      <c r="G25" s="133"/>
+      <c r="B25" s="152"/>
+      <c r="C25" s="134"/>
+      <c r="D25" s="152"/>
+      <c r="E25" s="133"/>
+      <c r="F25" s="133"/>
+      <c r="G25" s="134"/>
       <c r="H25" s="10"/>
       <c r="I25" s="23"/>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" s="10"/>
-      <c r="B26" s="151"/>
-      <c r="C26" s="133"/>
-      <c r="D26" s="151"/>
-      <c r="E26" s="132"/>
-      <c r="F26" s="132"/>
-      <c r="G26" s="133"/>
+      <c r="B26" s="152"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="152"/>
+      <c r="E26" s="133"/>
+      <c r="F26" s="133"/>
+      <c r="G26" s="134"/>
       <c r="H26" s="10"/>
       <c r="I26" s="23"/>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" s="10"/>
-      <c r="B27" s="151"/>
-      <c r="C27" s="133"/>
-      <c r="D27" s="151"/>
-      <c r="E27" s="132"/>
-      <c r="F27" s="132"/>
-      <c r="G27" s="133"/>
+      <c r="B27" s="152"/>
+      <c r="C27" s="134"/>
+      <c r="D27" s="152"/>
+      <c r="E27" s="133"/>
+      <c r="F27" s="133"/>
+      <c r="G27" s="134"/>
       <c r="H27" s="10"/>
       <c r="I27" s="23"/>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" s="10"/>
-      <c r="B28" s="151"/>
-      <c r="C28" s="133"/>
-      <c r="D28" s="151"/>
-      <c r="E28" s="132"/>
-      <c r="F28" s="132"/>
-      <c r="G28" s="133"/>
+      <c r="B28" s="152"/>
+      <c r="C28" s="134"/>
+      <c r="D28" s="152"/>
+      <c r="E28" s="133"/>
+      <c r="F28" s="133"/>
+      <c r="G28" s="134"/>
       <c r="H28" s="10"/>
       <c r="I28" s="23"/>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" s="10"/>
-      <c r="B29" s="151"/>
-      <c r="C29" s="133"/>
-      <c r="D29" s="151"/>
-      <c r="E29" s="132"/>
-      <c r="F29" s="132"/>
-      <c r="G29" s="133"/>
+      <c r="B29" s="152"/>
+      <c r="C29" s="134"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="133"/>
+      <c r="F29" s="133"/>
+      <c r="G29" s="134"/>
       <c r="H29" s="10"/>
       <c r="I29" s="23"/>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="10"/>
-      <c r="B30" s="151"/>
-      <c r="C30" s="133"/>
-      <c r="D30" s="151"/>
-      <c r="E30" s="132"/>
-      <c r="F30" s="132"/>
-      <c r="G30" s="133"/>
+      <c r="B30" s="152"/>
+      <c r="C30" s="134"/>
+      <c r="D30" s="152"/>
+      <c r="E30" s="133"/>
+      <c r="F30" s="133"/>
+      <c r="G30" s="134"/>
       <c r="H30" s="10"/>
       <c r="I30" s="23"/>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" s="10"/>
-      <c r="B31" s="151"/>
-      <c r="C31" s="133"/>
-      <c r="D31" s="151"/>
-      <c r="E31" s="132"/>
-      <c r="F31" s="132"/>
-      <c r="G31" s="133"/>
+      <c r="B31" s="152"/>
+      <c r="C31" s="134"/>
+      <c r="D31" s="152"/>
+      <c r="E31" s="133"/>
+      <c r="F31" s="133"/>
+      <c r="G31" s="134"/>
       <c r="H31" s="10"/>
       <c r="I31" s="23"/>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="10"/>
-      <c r="B32" s="151"/>
-      <c r="C32" s="133"/>
-      <c r="D32" s="151"/>
-      <c r="E32" s="132"/>
-      <c r="F32" s="132"/>
-      <c r="G32" s="133"/>
+      <c r="B32" s="152"/>
+      <c r="C32" s="134"/>
+      <c r="D32" s="152"/>
+      <c r="E32" s="133"/>
+      <c r="F32" s="133"/>
+      <c r="G32" s="134"/>
       <c r="H32" s="10"/>
       <c r="I32" s="23"/>
     </row>
     <row r="33" spans="1:9">
       <c r="A33" s="10"/>
-      <c r="B33" s="151"/>
-      <c r="C33" s="133"/>
-      <c r="D33" s="151"/>
-      <c r="E33" s="132"/>
-      <c r="F33" s="132"/>
-      <c r="G33" s="133"/>
+      <c r="B33" s="152"/>
+      <c r="C33" s="134"/>
+      <c r="D33" s="152"/>
+      <c r="E33" s="133"/>
+      <c r="F33" s="133"/>
+      <c r="G33" s="134"/>
       <c r="H33" s="10"/>
       <c r="I33" s="23"/>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="10"/>
-      <c r="B34" s="151"/>
-      <c r="C34" s="133"/>
-      <c r="D34" s="151"/>
-      <c r="E34" s="132"/>
-      <c r="F34" s="132"/>
-      <c r="G34" s="133"/>
+      <c r="B34" s="152"/>
+      <c r="C34" s="134"/>
+      <c r="D34" s="152"/>
+      <c r="E34" s="133"/>
+      <c r="F34" s="133"/>
+      <c r="G34" s="134"/>
       <c r="H34" s="10"/>
       <c r="I34" s="23"/>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" s="10"/>
-      <c r="B35" s="151"/>
-      <c r="C35" s="133"/>
-      <c r="D35" s="151"/>
-      <c r="E35" s="132"/>
-      <c r="F35" s="132"/>
-      <c r="G35" s="133"/>
+      <c r="B35" s="152"/>
+      <c r="C35" s="134"/>
+      <c r="D35" s="152"/>
+      <c r="E35" s="133"/>
+      <c r="F35" s="133"/>
+      <c r="G35" s="134"/>
       <c r="H35" s="10"/>
       <c r="I35" s="23"/>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" s="10"/>
-      <c r="B36" s="151"/>
-      <c r="C36" s="133"/>
-      <c r="D36" s="151"/>
-      <c r="E36" s="132"/>
-      <c r="F36" s="132"/>
-      <c r="G36" s="133"/>
+      <c r="B36" s="152"/>
+      <c r="C36" s="134"/>
+      <c r="D36" s="152"/>
+      <c r="E36" s="133"/>
+      <c r="F36" s="133"/>
+      <c r="G36" s="134"/>
       <c r="H36" s="10"/>
       <c r="I36" s="23"/>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" s="11"/>
-      <c r="B37" s="151"/>
-      <c r="C37" s="133"/>
-      <c r="D37" s="151"/>
-      <c r="E37" s="132"/>
-      <c r="F37" s="132"/>
-      <c r="G37" s="133"/>
+      <c r="B37" s="152"/>
+      <c r="C37" s="134"/>
+      <c r="D37" s="152"/>
+      <c r="E37" s="133"/>
+      <c r="F37" s="133"/>
+      <c r="G37" s="134"/>
       <c r="H37" s="11"/>
       <c r="I37" s="24"/>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="11"/>
-      <c r="B38" s="151"/>
-      <c r="C38" s="133"/>
-      <c r="D38" s="151"/>
-      <c r="E38" s="132"/>
-      <c r="F38" s="132"/>
-      <c r="G38" s="133"/>
+      <c r="B38" s="152"/>
+      <c r="C38" s="134"/>
+      <c r="D38" s="152"/>
+      <c r="E38" s="133"/>
+      <c r="F38" s="133"/>
+      <c r="G38" s="134"/>
       <c r="H38" s="11"/>
       <c r="I38" s="24"/>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="11"/>
-      <c r="B39" s="151"/>
-      <c r="C39" s="133"/>
-      <c r="D39" s="151"/>
-      <c r="E39" s="132"/>
-      <c r="F39" s="132"/>
-      <c r="G39" s="133"/>
+      <c r="B39" s="152"/>
+      <c r="C39" s="134"/>
+      <c r="D39" s="152"/>
+      <c r="E39" s="133"/>
+      <c r="F39" s="133"/>
+      <c r="G39" s="134"/>
       <c r="H39" s="11"/>
       <c r="I39" s="24"/>
     </row>
     <row r="40" spans="1:9">
       <c r="A40" s="11"/>
-      <c r="B40" s="151"/>
-      <c r="C40" s="133"/>
-      <c r="D40" s="151"/>
-      <c r="E40" s="132"/>
-      <c r="F40" s="132"/>
-      <c r="G40" s="133"/>
+      <c r="B40" s="152"/>
+      <c r="C40" s="134"/>
+      <c r="D40" s="152"/>
+      <c r="E40" s="133"/>
+      <c r="F40" s="133"/>
+      <c r="G40" s="134"/>
       <c r="H40" s="11"/>
       <c r="I40" s="24"/>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" s="11"/>
-      <c r="B41" s="151"/>
-      <c r="C41" s="133"/>
-      <c r="D41" s="151"/>
-      <c r="E41" s="132"/>
-      <c r="F41" s="132"/>
-      <c r="G41" s="133"/>
+      <c r="B41" s="152"/>
+      <c r="C41" s="134"/>
+      <c r="D41" s="152"/>
+      <c r="E41" s="133"/>
+      <c r="F41" s="133"/>
+      <c r="G41" s="134"/>
       <c r="H41" s="11"/>
       <c r="I41" s="24"/>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" s="12"/>
-      <c r="B42" s="152"/>
-      <c r="C42" s="153"/>
-      <c r="D42" s="152"/>
-      <c r="E42" s="154"/>
-      <c r="F42" s="154"/>
-      <c r="G42" s="153"/>
+      <c r="B42" s="153"/>
+      <c r="C42" s="154"/>
+      <c r="D42" s="153"/>
+      <c r="E42" s="155"/>
+      <c r="F42" s="155"/>
+      <c r="G42" s="154"/>
       <c r="H42" s="12"/>
       <c r="I42" s="25"/>
     </row>
@@ -7163,79 +7177,79 @@
       <c r="I43" s="20"/>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="148" t="s">
+      <c r="A44" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B44" s="149"/>
-      <c r="C44" s="149"/>
-      <c r="D44" s="149"/>
-      <c r="E44" s="149"/>
-      <c r="F44" s="149"/>
-      <c r="G44" s="149"/>
-      <c r="H44" s="149"/>
-      <c r="I44" s="150"/>
+      <c r="B44" s="150"/>
+      <c r="C44" s="150"/>
+      <c r="D44" s="150"/>
+      <c r="E44" s="150"/>
+      <c r="F44" s="150"/>
+      <c r="G44" s="150"/>
+      <c r="H44" s="150"/>
+      <c r="I44" s="151"/>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="148" t="s">
+      <c r="A45" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B45" s="149"/>
-      <c r="C45" s="149"/>
-      <c r="D45" s="149"/>
-      <c r="E45" s="149"/>
-      <c r="F45" s="149"/>
-      <c r="G45" s="149"/>
-      <c r="H45" s="149"/>
-      <c r="I45" s="150"/>
+      <c r="B45" s="150"/>
+      <c r="C45" s="150"/>
+      <c r="D45" s="150"/>
+      <c r="E45" s="150"/>
+      <c r="F45" s="150"/>
+      <c r="G45" s="150"/>
+      <c r="H45" s="150"/>
+      <c r="I45" s="151"/>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="148" t="s">
+      <c r="A46" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B46" s="149"/>
-      <c r="C46" s="149"/>
-      <c r="D46" s="149"/>
-      <c r="E46" s="149"/>
-      <c r="F46" s="149"/>
-      <c r="G46" s="149"/>
-      <c r="H46" s="149"/>
-      <c r="I46" s="150"/>
+      <c r="B46" s="150"/>
+      <c r="C46" s="150"/>
+      <c r="D46" s="150"/>
+      <c r="E46" s="150"/>
+      <c r="F46" s="150"/>
+      <c r="G46" s="150"/>
+      <c r="H46" s="150"/>
+      <c r="I46" s="151"/>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="148" t="s">
+      <c r="A47" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B47" s="149"/>
-      <c r="C47" s="149"/>
-      <c r="D47" s="149"/>
-      <c r="E47" s="149"/>
-      <c r="F47" s="149"/>
-      <c r="G47" s="149"/>
-      <c r="H47" s="149"/>
-      <c r="I47" s="150"/>
+      <c r="B47" s="150"/>
+      <c r="C47" s="150"/>
+      <c r="D47" s="150"/>
+      <c r="E47" s="150"/>
+      <c r="F47" s="150"/>
+      <c r="G47" s="150"/>
+      <c r="H47" s="150"/>
+      <c r="I47" s="151"/>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="148" t="s">
+      <c r="A48" s="149" t="s">
         <v>85</v>
       </c>
-      <c r="B48" s="149"/>
-      <c r="C48" s="149"/>
-      <c r="D48" s="149"/>
-      <c r="E48" s="149"/>
-      <c r="F48" s="149"/>
-      <c r="G48" s="149"/>
-      <c r="H48" s="149"/>
-      <c r="I48" s="150"/>
+      <c r="B48" s="150"/>
+      <c r="C48" s="150"/>
+      <c r="D48" s="150"/>
+      <c r="E48" s="150"/>
+      <c r="F48" s="150"/>
+      <c r="G48" s="150"/>
+      <c r="H48" s="150"/>
+      <c r="I48" s="151"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="7"/>
       <c r="B49" s="8"/>
-      <c r="C49" s="143"/>
-      <c r="D49" s="143"/>
-      <c r="E49" s="143"/>
-      <c r="F49" s="143"/>
-      <c r="G49" s="143"/>
-      <c r="H49" s="143"/>
+      <c r="C49" s="144"/>
+      <c r="D49" s="144"/>
+      <c r="E49" s="144"/>
+      <c r="F49" s="144"/>
+      <c r="G49" s="144"/>
+      <c r="H49" s="144"/>
       <c r="I49" s="22"/>
     </row>
     <row r="50" spans="1:9">
@@ -7251,10 +7265,10 @@
     </row>
     <row r="51" spans="1:9">
       <c r="A51" s="6"/>
-      <c r="B51" s="144" t="s">
+      <c r="B51" s="145" t="s">
         <v>86</v>
       </c>
-      <c r="C51" s="144"/>
+      <c r="C51" s="145"/>
       <c r="D51" s="3"/>
       <c r="E51" s="3"/>
       <c r="F51" s="3" t="s">
@@ -7270,53 +7284,53 @@
       <c r="A52" s="15" t="s">
         <v>88</v>
       </c>
-      <c r="B52" s="145"/>
-      <c r="C52" s="145"/>
-      <c r="D52" s="145"/>
+      <c r="B52" s="146"/>
+      <c r="C52" s="146"/>
+      <c r="D52" s="146"/>
       <c r="E52" s="1"/>
       <c r="F52" s="16"/>
       <c r="G52" s="17"/>
-      <c r="H52" s="146"/>
-      <c r="I52" s="147"/>
+      <c r="H52" s="147"/>
+      <c r="I52" s="148"/>
     </row>
     <row r="53" spans="1:9">
       <c r="A53" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="B53" s="131"/>
-      <c r="C53" s="131"/>
-      <c r="D53" s="131"/>
+      <c r="B53" s="132"/>
+      <c r="C53" s="132"/>
+      <c r="D53" s="132"/>
       <c r="E53" s="1"/>
       <c r="F53" s="19"/>
       <c r="G53" s="17"/>
-      <c r="H53" s="132"/>
-      <c r="I53" s="133"/>
+      <c r="H53" s="133"/>
+      <c r="I53" s="134"/>
     </row>
     <row r="54" spans="1:9">
       <c r="A54" s="18" t="s">
         <v>90</v>
       </c>
-      <c r="B54" s="131"/>
-      <c r="C54" s="131"/>
-      <c r="D54" s="131"/>
+      <c r="B54" s="132"/>
+      <c r="C54" s="132"/>
+      <c r="D54" s="132"/>
       <c r="E54" s="1"/>
       <c r="F54" s="19"/>
       <c r="G54" s="17"/>
-      <c r="H54" s="132"/>
-      <c r="I54" s="133"/>
+      <c r="H54" s="133"/>
+      <c r="I54" s="134"/>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" s="18" t="s">
         <v>91</v>
       </c>
-      <c r="B55" s="131"/>
-      <c r="C55" s="131"/>
-      <c r="D55" s="131"/>
+      <c r="B55" s="132"/>
+      <c r="C55" s="132"/>
+      <c r="D55" s="132"/>
       <c r="E55" s="1"/>
       <c r="F55" s="19"/>
       <c r="G55" s="17"/>
-      <c r="H55" s="132"/>
-      <c r="I55" s="133"/>
+      <c r="H55" s="133"/>
+      <c r="I55" s="134"/>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" s="7"/>

</xml_diff>